<commit_message>
Updated app.py and index.html with BeautifulSoup and loader fix
</commit_message>
<xml_diff>
--- a/uploads/products.xlsx
+++ b/uploads/products.xlsx
@@ -11,51 +11,360 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="118">
   <si>
     <t>posDescription</t>
   </si>
   <si>
-    <t>Lamb</t>
-  </si>
-  <si>
-    <t>BASIL SEEDS DRINK</t>
-  </si>
-  <si>
-    <t>STUFFED GRAPED LEAVES</t>
-  </si>
-  <si>
-    <t>EGGS</t>
-  </si>
-  <si>
-    <t>GOLDEN BAKING DATES</t>
-  </si>
-  <si>
-    <t>NAMI JUICE</t>
-  </si>
-  <si>
-    <t>clover honey</t>
-  </si>
-  <si>
-    <t>HONEY</t>
-  </si>
-  <si>
-    <t>HONEY TURKISH</t>
-  </si>
-  <si>
-    <t>TUNISIAN DATES</t>
+    <t>CHICK  PEAS</t>
+  </si>
+  <si>
+    <t>HUMMUS CLASSIC</t>
+  </si>
+  <si>
+    <t>ALIEPPO HUMMUS</t>
+  </si>
+  <si>
+    <t>HUMMUS</t>
+  </si>
+  <si>
+    <t>BABAGANOUSH</t>
+  </si>
+  <si>
+    <t>OLIVE OIL</t>
+  </si>
+  <si>
+    <t>GRAPE SEEDS OIL</t>
+  </si>
+  <si>
+    <t>AVOADO OIL</t>
+  </si>
+  <si>
+    <t>FREEKEH</t>
+  </si>
+  <si>
+    <t>YOUGURT DRINK</t>
+  </si>
+  <si>
+    <t>PAN</t>
+  </si>
+  <si>
+    <t>FRIED ONION</t>
+  </si>
+  <si>
+    <t>PARS</t>
+  </si>
+  <si>
+    <t>Gaimar Sarshir</t>
+  </si>
+  <si>
+    <t>FIGS</t>
+  </si>
+  <si>
+    <t>TURKISH FIGS</t>
+  </si>
+  <si>
+    <t>TENDER POPS</t>
+  </si>
+  <si>
+    <t>tender pops</t>
+  </si>
+  <si>
+    <t>NUGGETS</t>
+  </si>
+  <si>
+    <t>FUN NUGGETS</t>
+  </si>
+  <si>
+    <t>nuggets</t>
+  </si>
+  <si>
+    <t>K&amp;NS SEEKH KABAB</t>
+  </si>
+  <si>
+    <t>WINGS</t>
+  </si>
+  <si>
+    <t>ASATEER BAKLAWA</t>
+  </si>
+  <si>
+    <t>BARAZEK</t>
+  </si>
+  <si>
+    <t>NUTS</t>
+  </si>
+  <si>
+    <t>WALNUT</t>
+  </si>
+  <si>
+    <t>GREEN RAISINS</t>
+  </si>
+  <si>
+    <t>pistachios</t>
+  </si>
+  <si>
+    <t>CHILI PEANUTS</t>
+  </si>
+  <si>
+    <t>ALMONSD</t>
+  </si>
+  <si>
+    <t>GOLDEN PRUNE</t>
+  </si>
+  <si>
+    <t>CHILI MANGO</t>
+  </si>
+  <si>
+    <t>SLICED APRICOT</t>
+  </si>
+  <si>
+    <t>BERIIES</t>
+  </si>
+  <si>
+    <t>ALMOND</t>
+  </si>
+  <si>
+    <t>BLACK RAISINS</t>
+  </si>
+  <si>
+    <t>CASHEWS</t>
+  </si>
+  <si>
+    <t>WHITE MULBERRY</t>
+  </si>
+  <si>
+    <t>PISTACHIOS</t>
+  </si>
+  <si>
+    <t>CRWAY SEED</t>
+  </si>
+  <si>
+    <t>FIGS NATURAL</t>
+  </si>
+  <si>
+    <t>SEDS</t>
+  </si>
+  <si>
+    <t>COCONUT CHIPS</t>
+  </si>
+  <si>
+    <t>PRUNE</t>
+  </si>
+  <si>
+    <t>CARDAMOM</t>
+  </si>
+  <si>
+    <t>DRIED CHERRIES</t>
+  </si>
+  <si>
+    <t>DRIED APRICOT</t>
+  </si>
+  <si>
+    <t>DRIED OLEASTER</t>
+  </si>
+  <si>
+    <t>SEEDS</t>
+  </si>
+  <si>
+    <t>RAISINS</t>
+  </si>
+  <si>
+    <t>MUNAKKA</t>
+  </si>
+  <si>
+    <t>CHICPEAS</t>
+  </si>
+  <si>
+    <t>SAFFRON ROCK CANDY</t>
+  </si>
+  <si>
+    <t>FANCY ROCK CANDY</t>
+  </si>
+  <si>
+    <t>MANGO</t>
+  </si>
+  <si>
+    <t>RAISINS RED</t>
+  </si>
+  <si>
+    <t>MLUBERRY</t>
+  </si>
+  <si>
+    <t>GAZ</t>
+  </si>
+  <si>
+    <t>PMPKIN SEEDS</t>
+  </si>
+  <si>
+    <t>GOJI</t>
+  </si>
+  <si>
+    <t>DATES</t>
+  </si>
+  <si>
+    <t>YELLOW POPCORN</t>
+  </si>
+  <si>
+    <t>FRUIT MIX</t>
+  </si>
+  <si>
+    <t>PUMPKIN SEED</t>
+  </si>
+  <si>
+    <t>OKRA CHIPS</t>
+  </si>
+  <si>
+    <t>CHILLI LMN</t>
+  </si>
+  <si>
+    <t>DRIED CANBERRIES</t>
+  </si>
+  <si>
+    <t>WALNUT  &amp; MULBERYY</t>
+  </si>
+  <si>
+    <t>TRAIL</t>
+  </si>
+  <si>
+    <t>GREEN PISTACHIOS</t>
+  </si>
+  <si>
+    <t>PINENUT IN SHELL</t>
+  </si>
+  <si>
+    <t>HARISSA</t>
+  </si>
+  <si>
+    <t>dates</t>
+  </si>
+  <si>
+    <t>TAZAH DATES</t>
+  </si>
+  <si>
+    <t>OUSCOUS</t>
   </si>
   <si>
     <t>PASTA</t>
   </si>
   <si>
-    <t>BAKING POWDER</t>
-  </si>
-  <si>
-    <t>NUTS</t>
-  </si>
-  <si>
-    <t>PRUNE</t>
+    <t>SWEETIES</t>
+  </si>
+  <si>
+    <t>BONART  DATES</t>
+  </si>
+  <si>
+    <t>PITTED DATES</t>
+  </si>
+  <si>
+    <t>DATE SYRUP</t>
+  </si>
+  <si>
+    <t>PITA</t>
+  </si>
+  <si>
+    <t>Balsimc Vinegar</t>
+  </si>
+  <si>
+    <t>EXTRA VIRGIN OLIVE OIL</t>
+  </si>
+  <si>
+    <t>LIME</t>
+  </si>
+  <si>
+    <t>LEMON</t>
+  </si>
+  <si>
+    <t>ZEITUN</t>
+  </si>
+  <si>
+    <t>ENNIO GRAPE SEE OIL</t>
+  </si>
+  <si>
+    <t>LIQUID SAFRON</t>
+  </si>
+  <si>
+    <t>ENNIO OLIVE OIL</t>
+  </si>
+  <si>
+    <t>OLIVE OIL GAGLIO</t>
+  </si>
+  <si>
+    <t>DELLI MEAT</t>
+  </si>
+  <si>
+    <t>HAZELNUT BISCOTTI</t>
+  </si>
+  <si>
+    <t>CHOCOLATE BISCOTTI</t>
+  </si>
+  <si>
+    <t>ALMOND BISCOTTI</t>
+  </si>
+  <si>
+    <t>SAFFRON BISCOTTI</t>
+  </si>
+  <si>
+    <t>COMB HONE AMOROSSI</t>
+  </si>
+  <si>
+    <t>FIFI'S SWEET</t>
+  </si>
+  <si>
+    <t>RASPBERRY COOKIES</t>
+  </si>
+  <si>
+    <t>APRICOT COOKIES</t>
+  </si>
+  <si>
+    <t>AMOROSI HONEY</t>
+  </si>
+  <si>
+    <t>FIFI'S VANILA ALMOND COOKIES</t>
+  </si>
+  <si>
+    <t>ABRAHAM BAKE</t>
+  </si>
+  <si>
+    <t>ABRAHAM BAKERY RAISIN COOKY</t>
+  </si>
+  <si>
+    <t>DATE ROLLS</t>
+  </si>
+  <si>
+    <t>SUKKARI</t>
+  </si>
+  <si>
+    <t>SUFRI</t>
+  </si>
+  <si>
+    <t>CHEESE</t>
+  </si>
+  <si>
+    <t>YOREM</t>
+  </si>
+  <si>
+    <t>LABNE</t>
+  </si>
+  <si>
+    <t>KASAR TAZA</t>
+  </si>
+  <si>
+    <t>SELE OLIVES</t>
+  </si>
+  <si>
+    <t>OLIVES</t>
+  </si>
+  <si>
+    <t>olive</t>
+  </si>
+  <si>
+    <t>RICE</t>
+  </si>
+  <si>
+    <t>Yorem</t>
+  </si>
+  <si>
+    <t>ULKER</t>
   </si>
 </sst>
 </file>
@@ -111,7 +420,7 @@
       <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
@@ -359,52 +668,877 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>